<commit_message>
Update fitur login dan registrasi + update data user/kendaraan
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,14 +582,51 @@
           <t>Palembang</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>70000</v>
-      </c>
-      <c r="F5" s="2" t="n">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>70000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2026-07-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>70000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2345678990112444</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BG6701HI</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Tiara</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>90000</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>46233</v>
       </c>
-      <c r="G5" t="n">
-        <v>70000</v>
+      <c r="G6" t="n">
+        <v>90000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tambahkan data awal pengguna dan kendaraan
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,14 +619,88 @@
           <t>Palembang</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>90000</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>46233</v>
-      </c>
-      <c r="G6" t="n">
-        <v>90000</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>90000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2026-07-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>90000</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1245367800112234</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BG7783GI</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Sinta Maharani</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2026-07-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>9801234567819235</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BG8799BI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Dinda</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>80000</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>46234</v>
+      </c>
+      <c r="G8" t="n">
+        <v>80000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update riwayat pembayaran dan logika pembayaran terakhir
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +469,11 @@
           <t>Pajak</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -506,6 +507,7 @@
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -539,6 +541,7 @@
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -560,6 +563,7 @@
           <t>50000</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -597,6 +601,7 @@
           <t>70000</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -634,6 +639,11 @@
           <t>90000</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>LUNAS</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -671,6 +681,7 @@
           <t>40000</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -693,15 +704,22 @@
           <t>Palembang</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>80000</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>46234</v>
-      </c>
-      <c r="G8" t="n">
-        <v>80000</v>
-      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>80000</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2026-07-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>80000</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update data kendaraan dan riwayat pembayaran
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -601,7 +601,11 @@
           <t>70000</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>LUNAS</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">

</xml_diff>

<commit_message>
Update fitur statistik pribadi dan visualisasi
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -723,7 +723,11 @@
           <t>80000</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>LUNAS</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update: fix login & tampilkan data profil + kendaraan, perbaikan format pajak
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,26 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>Nomor_Rangka</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Merek</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Warna</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Status</t>
         </is>
       </c>
@@ -478,17 +498,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1234567890123450</t>
+          <t>1234456278949542</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BG1234XY</t>
+          <t>BG4576HI</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Andi</t>
+          <t>Nia Rahmadani</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -498,232 +518,40 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>550000</t>
+          <t>65000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-08-30 00:00:00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>3201234567890000</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BG5678AB</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Budi</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Palembang</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>780000</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2025-09-15 00:00:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>12345678900000</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>BG9876UI</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>50000</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1234456278949542</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>BG4576HI</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Nia</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Palembang</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>70000</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2026-07-30 00:00:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>70000</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>LUNAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2345678990112444</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>BG6701HI</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Tiara</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Palembang</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>90000</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2026-07-30 00:00:00</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>90000</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>LUNAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>1245367800112234</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>BG7783GI</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Sinta Maharani</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Palembang</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>40000</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2026-07-31 00:00:00</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>40000</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>9801234567819235</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>BG8799BI</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Dinda</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Palembang</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>80000</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2026-07-31 00:00:00</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>80000</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
+          <t>2026-08-02 00:00:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NMR123XYZ</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Honda</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Sepeda Motor</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Biru</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>LUNAS</t>
         </is>

</xml_diff>

<commit_message>
✅ Tambah fitur cetak resi, otomatis status pengiriman, dan PDF download
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,21 @@
           <t>Status</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Status_Pengiriman</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>No_Resi</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Ekspedisi</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -554,6 +569,21 @@
       <c r="L2" t="inlineStr">
         <is>
           <t>LUNAS</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Diproses</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>RESI426356</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>J&amp;T</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
✨ Tambah status pengiriman & tampilan tabel berwarna
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -578,12 +578,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>RESI426356</t>
+          <t>RESI815663</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>J&amp;T</t>
+          <t>JNE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update data_user, data_kendaraan, dan fungsi utils
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +591,61 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1234456278949533</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BG6744HU</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Rahma</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>65000</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>46240</v>
+      </c>
+      <c r="G3" t="n">
+        <v>65000</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>HIDJR3544H</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Yamaha</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Sepeda Motor</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Hitam</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Perbaikan lebar tampilan profil + update data kendaraan dan user
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/data_kendaraan.xlsx
+++ b/DASHBOARD_main/data_kendaraan.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,14 +612,20 @@
           <t>Palembang</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>65000</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>46240</v>
-      </c>
-      <c r="G3" t="n">
-        <v>65000</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2026-08-06 00:00:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -646,6 +652,61 @@
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>7868866666665555</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BG8989HI</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Siti Aminah</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>65000</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>46240</v>
+      </c>
+      <c r="G4" t="n">
+        <v>65000</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>MKK89JKK</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Honda</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Sepeda Motor</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Hitam</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>